<commit_message>
7334: Fixed math in extract_qb_data specs
</commit_message>
<xml_diff>
--- a/docs/example_calculation.xlsx
+++ b/docs/example_calculation.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6880" yWindow="22060" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="12120" yWindow="29260" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -95,9 +95,6 @@
     <t>Int inc</t>
   </si>
   <si>
-    <t>Int recv</t>
-  </si>
-  <si>
     <t>Prin</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>Second payout of $52.50</t>
+  </si>
+  <si>
+    <t>Int rcv</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,19 +464,19 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>21</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -841,7 +841,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="O12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>